<commit_message>
Added db file and formatted the database format
</commit_message>
<xml_diff>
--- a/Student DB.xlsx
+++ b/Student DB.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Enrollment No.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -40,13 +37,19 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>University Roll Number.</t>
+  </si>
+  <si>
+    <t>University Registration Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -181,7 +184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -358,53 +361,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the database format
</commit_message>
<xml_diff>
--- a/Student DB.xlsx
+++ b/Student DB.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Enrollment No.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +37,15 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>University Roll Number</t>
+  </si>
+  <si>
+    <t>University Registration Number</t>
   </si>
 </sst>
 </file>
@@ -366,45 +372,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.21875" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added database and tables
</commit_message>
<xml_diff>
--- a/Student DB.xlsx
+++ b/Student DB.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
@@ -10,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -105,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,33 +418,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="37.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -452,7 +452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -462,23 +462,23 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -488,23 +488,23 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -512,7 +512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -520,7 +520,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18">
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -531,12 +531,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -547,7 +547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>

</xml_diff>